<commit_message>
More comments added to the open API Specification (CCBS_API.json). Minor corrections to the excel files
</commit_message>
<xml_diff>
--- a/IA_CCBS_BANK_SIDE/Position/Exposures_DownloadPosition.xlsx
+++ b/IA_CCBS_BANK_SIDE/Position/Exposures_DownloadPosition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aafent\Desktop\IA\Interfaces\IA_CCBS_BANK_SIDE\Position\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aafent\Desktop\IA\InterfacesGitHub\IA_CCBS_BANK_SIDE\Position\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79916BC3-294B-431B-944C-5E30E6AD3088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEB1F48-DFF6-40A1-A46D-AE9690405D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7800" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{9E1DAA95-CF3D-4818-92B3-96838C995953}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{9E1DAA95-CF3D-4818-92B3-96838C995953}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -249,9 +249,6 @@
     <t>cb_lastinstamt</t>
   </si>
   <si>
-    <t>If amount27 is zero then amount23</t>
-  </si>
-  <si>
     <t>Not Used</t>
   </si>
   <si>
@@ -342,6 +339,9 @@
   </si>
   <si>
     <t>i-Apply</t>
+  </si>
+  <si>
+    <t>the maximun amount to be paied (future installments), If amount27 is zero then amount23</t>
   </si>
 </sst>
 </file>
@@ -1054,9 +1054,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1094,7 +1094,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1200,7 +1200,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1342,7 +1342,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1359,100 +1359,100 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" style="25" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="59.42578125" style="25" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="25"/>
+    <col min="2" max="2" width="17.44140625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" style="25" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="25"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="27" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="28" t="s">
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="27" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
-        <v>82</v>
-      </c>
       <c r="C4" s="28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="28" t="s">
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="27" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
+      <c r="C6" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="27"/>
       <c r="C7" s="28"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="27"/>
       <c r="C9" s="28"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C11" s="28" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="27"/>
       <c r="C12" s="28"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="27"/>
       <c r="C13" s="28"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="28" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
     </row>
@@ -1465,43 +1465,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95117F95-D086-4AAA-9DF4-E07FFE825B20}">
   <dimension ref="B2:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="28.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="2"/>
+    <col min="3" max="3" width="28.5546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="43.5703125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="16.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="43.5546875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>96</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>97</v>
       </c>
       <c r="F2" s="30" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24">
         <v>1</v>
       </c>
@@ -1519,7 +1519,7 @@
       </c>
       <c r="G3" s="20"/>
     </row>
-    <row r="4" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24">
         <v>2</v>
       </c>
@@ -1537,492 +1537,492 @@
       </c>
       <c r="G4" s="23"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="32"/>
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
-    <row r="29" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C29" s="32"/>
       <c r="D29" s="9"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="32"/>
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="32"/>
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
     </row>
-    <row r="32" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C32" s="32"/>
       <c r="D32" s="9"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
     </row>
-    <row r="33" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="32"/>
       <c r="D33" s="9"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="3:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
     </row>
-    <row r="38" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
     </row>
-    <row r="40" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
     </row>
-    <row r="41" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
     </row>
-    <row r="48" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
     </row>
-    <row r="79" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
       <c r="E79" s="12"/>
       <c r="F79" s="12"/>
     </row>
-    <row r="80" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
     </row>
-    <row r="81" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
     </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
     </row>
-    <row r="84" spans="3:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:6" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="6"/>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="6"/>
       <c r="F85" s="6"/>
     </row>
-    <row r="87" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:6" x14ac:dyDescent="0.3">
       <c r="E87" s="17"/>
     </row>
   </sheetData>
@@ -2042,32 +2042,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D9F46F-6418-4AAF-BC4D-845CE01B7A50}">
   <dimension ref="B2:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="26"/>
-    <col min="3" max="3" width="27.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="26"/>
+    <col min="3" max="3" width="27.109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" style="25" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" style="25" customWidth="1"/>
     <col min="6" max="6" width="17" style="25" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="144.7109375" style="25" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="25"/>
+    <col min="7" max="7" width="12.6640625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="144.6640625" style="25" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="25"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>1</v>
@@ -2079,10 +2079,10 @@
         <v>3</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="26">
         <v>1</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="26">
         <v>2</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="26">
         <v>3</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="26">
         <v>4</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="26">
         <v>5</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="26">
         <v>6</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="26">
         <v>7</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="26">
         <v>8</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="26">
         <v>9</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="26">
         <v>10</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="26">
         <v>11</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="26">
         <v>12</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="26">
         <v>13</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="26">
         <v>14</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="26">
         <v>15</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="26">
         <v>16</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="26">
         <v>17</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="26">
         <v>18</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="26">
         <v>19</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="26">
         <v>20</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="26">
         <v>21</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="26">
         <v>22</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="26">
         <v>23</v>
       </c>
@@ -2413,69 +2413,69 @@
         <v>38</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="26">
         <v>24</v>
       </c>
       <c r="C26" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="25" t="s">
         <v>68</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>69</v>
       </c>
       <c r="F26" s="25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="26">
         <v>25</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="26">
         <v>26</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F28" s="25" t="s">
         <v>7</v>
       </c>
       <c r="H28" s="25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="26">
         <v>27</v>
       </c>
       <c r="C29" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>75</v>
       </c>
       <c r="F29" s="25" t="s">
         <v>28</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>